<commit_message>
biotic and abiotic variables
</commit_message>
<xml_diff>
--- a/experiments-structure.xlsx
+++ b/experiments-structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbfaa4602b6a5992/Academicos/R/Workspace/huberi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="280" documentId="113_{A031EB86-9DB2-459C-B4DC-FC9D31340DBC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{88744C71-8DC3-E241-B8F4-B1E63DCFE753}"/>
+  <xr:revisionPtr revIDLastSave="700" documentId="113_{A031EB86-9DB2-459C-B4DC-FC9D31340DBC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{876654BF-FC98-2C47-BAA4-9FA19CE9B195}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="900" windowWidth="27320" windowHeight="15360" xr2:uid="{9C35A8F3-3922-9F4C-8370-7246F424F389}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9C35A8F3-3922-9F4C-8370-7246F424F389}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="128">
   <si>
     <t>métodos</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Input</t>
-  </si>
-  <si>
-    <t>climáticas ( 5 vars ) + SOLO (PLANTAS)</t>
   </si>
   <si>
     <t>Resposta</t>
@@ -147,8 +144,396 @@
     <t xml:space="preserve"> RecursoSUIT</t>
   </si>
   <si>
+    <t>Presente + Futuro - 4 RCPs</t>
+  </si>
+  <si>
+    <t>Fase1</t>
+  </si>
+  <si>
+    <t>Fase 2</t>
+  </si>
+  <si>
+    <t>Ensemble Presente | Se for o mais representativo + 4 Ensembles (Futuro)</t>
+  </si>
+  <si>
+    <t>De XP2 a XP7  analisaremos sómente o mais representatativo no presente</t>
+  </si>
+  <si>
+    <t>resposta: huberi</t>
+  </si>
+  <si>
+    <t>preditor: adequabilidade ponderada XP2:XP7</t>
+  </si>
+  <si>
+    <t>FASE 2 - Escolha do XP</t>
+  </si>
+  <si>
+    <t>AVALIAÇAO DA REPRESENTATIVIDADE</t>
+  </si>
+  <si>
+    <t>Anova de Medidas Repetidas (mesmos subconjuntos de XP2 a XP7)</t>
+  </si>
+  <si>
+    <t>preditor: tamanho de range  XP2:XP7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gera Variávies Preditoras</t>
+  </si>
+  <si>
+    <t>EXPERIMENTOS</t>
+  </si>
+  <si>
+    <t>Preditora Biótica</t>
+  </si>
+  <si>
+    <t>SEP/SUIT</t>
+  </si>
+  <si>
+    <t>STK/SUIT</t>
+  </si>
+  <si>
+    <t>SEP/PA***</t>
+  </si>
+  <si>
+    <t>STK/PA****</t>
+  </si>
+  <si>
+    <t>1. Criaçao variáveis bióticas preditoras em XP1</t>
+  </si>
+  <si>
+    <t>2. Matriz de Presença e Ausência - Limiar de corte</t>
+  </si>
+  <si>
+    <t>3. Checar a função Multiple_ENMs</t>
+  </si>
+  <si>
+    <t>4. Criaçao Ensembles multiplos para XP1  9 espécies</t>
+  </si>
+  <si>
+    <t>resposta: huberi (mesma resposta dividida nos mesmos subgrupos %treino/%teste no 6 XPs)</t>
+  </si>
+  <si>
+    <t>5. Avaliaçao de representatividade. ANOREP. Preparaçao de fatores.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Preparaçao de fatores para Ensemble / Análise de incerteza para </t>
+  </si>
+  <si>
+    <t>Duvidas duvidosas</t>
+  </si>
+  <si>
+    <t>resourcePA_c,</t>
+  </si>
+  <si>
+    <t>resouceSUIT_c,</t>
+  </si>
+  <si>
+    <t>resourcePA_rcp26,</t>
+  </si>
+  <si>
+    <t>resouceSUIT_rcp26,</t>
+  </si>
+  <si>
+    <t>resourcePA_rcp45,</t>
+  </si>
+  <si>
+    <t>resouceSUIT_rcp45,</t>
+  </si>
+  <si>
+    <t>resourcePA_rcp60,</t>
+  </si>
+  <si>
+    <t>resouceSUIT_rcp60,</t>
+  </si>
+  <si>
+    <t>resourcePA_rcp85,</t>
+  </si>
+  <si>
+    <t>resouceSUIT_rcp85,</t>
+  </si>
+  <si>
+    <t>BIÓTICAS</t>
+  </si>
+  <si>
+    <t>VARS</t>
+  </si>
+  <si>
+    <t>rcp26</t>
+  </si>
+  <si>
+    <t>rcp45</t>
+  </si>
+  <si>
+    <t>rcp60</t>
+  </si>
+  <si>
+    <t>rcp85</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>ABIÓTICAS</t>
+  </si>
+  <si>
+    <t>7. EM XP1 inlcuir SOLO somente para plantas - ABORTADO PARA DEFESA. EMPLEMENTAR PARA PUBLICAÇAO</t>
+  </si>
+  <si>
+    <t>SEP_PA_c,</t>
+  </si>
+  <si>
+    <t>SEP_PA_rcp26,</t>
+  </si>
+  <si>
+    <t>SEP_PA_rcp45,</t>
+  </si>
+  <si>
+    <t>SEP_PA_rcp60,</t>
+  </si>
+  <si>
+    <t>SEP_PA_rcp85,</t>
+  </si>
+  <si>
+    <t>SEP_SUIT_c,</t>
+  </si>
+  <si>
+    <t>SEP_SUIT_rcp26,</t>
+  </si>
+  <si>
+    <t>SEP_SUIT_rcp45,</t>
+  </si>
+  <si>
+    <t>SEP_SUIT_rcp60,</t>
+  </si>
+  <si>
+    <t>SEP_SUIT_rcp85,</t>
+  </si>
+  <si>
+    <t>STK_PA_c,</t>
+  </si>
+  <si>
+    <t>STK_PA_rcp26,</t>
+  </si>
+  <si>
+    <t>STK_PA_rcp45,</t>
+  </si>
+  <si>
+    <t>STK_PA_rcp60,</t>
+  </si>
+  <si>
+    <t>STK_PA_rcp85,</t>
+  </si>
+  <si>
+    <t>STK_SUIT_c,</t>
+  </si>
+  <si>
+    <t>STK_SUIT_rcp26,</t>
+  </si>
+  <si>
+    <t>STK_SUIT_rcp45,</t>
+  </si>
+  <si>
+    <t>STK_SUIT_rcp60,</t>
+  </si>
+  <si>
+    <t>STK_SUIT_rcp85,</t>
+  </si>
+  <si>
+    <t>ABIÓTICAS 
+utilizadas em XP1</t>
+  </si>
+  <si>
+    <t>INPUT</t>
+  </si>
+  <si>
+    <t>NEW VARS</t>
+  </si>
+  <si>
+    <t>ABELHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRESENTE 
++ 
+4 RCPS X 3 AOGCMS
+</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>sep_pa</t>
+  </si>
+  <si>
+    <t>sep_suit</t>
+  </si>
+  <si>
+    <t>stk_pa</t>
+  </si>
+  <si>
+    <t>stk_suit</t>
+  </si>
+  <si>
+    <t>recurso_pa</t>
+  </si>
+  <si>
+    <t>recurso_suit</t>
+  </si>
+  <si>
+    <t>c, 26, 45, 60, 85</t>
+  </si>
+  <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>biótica</t>
+  </si>
+  <si>
+    <t>CLIMA_CURRENT
+CLIMA_RCP26
+CLIMA_RCP45
+CLIMA_RCP60
+CLIMA_RCP85</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>7 PLANTAS</t>
+  </si>
+  <si>
+    <t>"RECURSO"</t>
+  </si>
+  <si>
+    <t>* somente as plantas sáo 
+utilizadas para gerar as
+novas variaveis</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">CLIMÁTICAS + </t>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Corpo)_x0000_"/>
+      </rPr>
+      <t>ABIÓTICAS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  ( 5 vars ) + SOLO (PLANTAS)</t>
+    </r>
+  </si>
+  <si>
+    <t>VARIÁVEIS BIÓTICAS GERADAS COM INPUTS DAS PLANTAS</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Corpo)_x0000_"/>
+      </rPr>
+      <t>BIÓTICAS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - SEP/PA -  (13 vars = 5  + 8 )</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Corpo)_x0000_"/>
+      </rPr>
+      <t>BIÓTICAS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - SEP/SUIT -   (12 vars =  5  + 7 )</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Corpo)_x0000_"/>
+      </rPr>
+      <t>BIÓTICAS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - STK/PA -  (6 vars = 5  + 1 ) média ou soma dos mapas PA das plantas</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Corpo)_x0000_"/>
+      </rPr>
+      <t>BIÓTICAS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - STK/SUIT - (6 vars = 5  +  1 ) *média  ou soma das suitabilities dos Ensenbles?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Corpo)_x0000_"/>
+      </rPr>
+      <t>BIÓTICAS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
     </r>
     <r>
       <rPr>
@@ -172,7 +557,23 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">CLIMÁTICAS + </t>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Corpo)_x0000_"/>
+      </rPr>
+      <t>BIÓTICAS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -  </t>
     </r>
     <r>
       <rPr>
@@ -195,13 +596,10 @@
     </r>
   </si>
   <si>
-    <t>Presente + Futuro - 4 RCPs</t>
-  </si>
-  <si>
     <r>
       <rPr>
+        <b/>
         <sz val="12"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri (Corpo)_x0000_"/>
       </rPr>
       <t>Presente</t>
@@ -218,130 +616,19 @@
     </r>
   </si>
   <si>
-    <t>Fase1</t>
-  </si>
-  <si>
-    <t>Fase 2</t>
-  </si>
-  <si>
-    <t>9 Ensembles - média ponderada  das suit  dos 4 modelos tendo como peso a estatística d**</t>
-  </si>
-  <si>
-    <t>Ensemble Presente | Se for o mais representativo + 4 Ensembles (Futuro)</t>
-  </si>
-  <si>
-    <t>De XP2 a XP7  analisaremos sómente o mais representatativo no presente</t>
-  </si>
-  <si>
-    <t>resposta: huberi</t>
-  </si>
-  <si>
-    <t>preditor: adequabilidade ponderada XP2:XP7</t>
-  </si>
-  <si>
-    <t>FASE 2 - Escolha do XP</t>
-  </si>
-  <si>
-    <t>AVALIAÇAO DA REPRESENTATIVIDADE</t>
-  </si>
-  <si>
-    <t>Anova de Medidas Repetidas (mesmos subconjuntos de XP2 a XP7)</t>
-  </si>
-  <si>
-    <t>preditor: tamanho de range  XP2:XP7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gera Variávies Preditoras</t>
-  </si>
-  <si>
-    <t>EXPERIMENTOS</t>
-  </si>
-  <si>
-    <t>Preditora Biótica</t>
-  </si>
-  <si>
-    <t>SEP/SUIT</t>
-  </si>
-  <si>
-    <t>STK/SUIT</t>
-  </si>
-  <si>
-    <t>CLIMÁTICAS + SEP/PA -  (12 vars = 5  + 7 )</t>
-  </si>
-  <si>
-    <t>CLIMÁTICAS + SEP/SUIT -   (12 vars =  5  + 7 )</t>
-  </si>
-  <si>
-    <r>
-      <t>CLIMÁTICAS +</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>STK/PA -  (6 vars = 5  + 1 ) somatório dos mapas PA das plantas</t>
-    </r>
-  </si>
-  <si>
-    <t>CLIMÁTICAS + STK/SUIT - (6 vars = 5  +  1 ) *média  ou soma das suitabilities dos Ensenbles? Talvez fazer outro XP  para considerar ambos?</t>
-  </si>
-  <si>
-    <t>SEP/PA***</t>
-  </si>
-  <si>
-    <t>STK/PA****</t>
-  </si>
-  <si>
-    <t>1. Criaçao variáveis bióticas preditoras em XP1</t>
-  </si>
-  <si>
-    <t>2. Matriz de Presença e Ausência - Limiar de corte</t>
-  </si>
-  <si>
-    <t>3. Checar a função Multiple_ENMs</t>
-  </si>
-  <si>
-    <t>4. Criaçao Ensembles multiplos para XP1  9 espécies</t>
-  </si>
-  <si>
-    <t>resposta: huberi (mesma resposta dividida nos mesmos subgrupos %treino/%teste no 6 XPs)</t>
-  </si>
-  <si>
-    <t>5. Avaliaçao de representatividade. ANOREP. Preparaçao de fatores.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6. Preparaçao de fatores para Ensemble / Análise de incerteza para </t>
-  </si>
-  <si>
-    <t>7. EM XP1 inlcuir SOLO somente para plantas</t>
-  </si>
-  <si>
-    <t>8. COMO modelar com mais de uma variável, CLIMÁTICAS + BIÓTICA? Não penso que seria em um mesmo objeto.</t>
-  </si>
-  <si>
-    <t>Duvidas duvidosas</t>
+    <t>BIÓTICAS
+utilizadas 
+de XP2 a XP7</t>
+  </si>
+  <si>
+    <t>8. VARIÁVEIS ABIÓTICAS SÓ EM XP1 E VARIÁVIES BIÓTICAS DE XP2 A XP7. ESTOU CORRETO?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -372,24 +659,11 @@
       <name val="Calibri (Corpo)_x0000_"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF2600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri (Corpo)_x0000_"/>
     </font>
     <font>
       <b/>
@@ -407,8 +681,70 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri (Corpo)_x0000_"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri (Corpo)_x0000_"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri (Corpo)_x0000_"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,10 +775,97 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -452,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -461,12 +884,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -475,8 +897,122 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,49 +1327,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813E66E3-DA6A-6A4C-AE0E-7BACBC27F508}">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:AC66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G21" zoomScale="171" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D21" zoomScale="109" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="4.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" customWidth="1"/>
+    <col min="9" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" customWidth="1"/>
+    <col min="21" max="21" width="16" customWidth="1"/>
+    <col min="22" max="22" width="17" customWidth="1"/>
+    <col min="24" max="24" width="17.83203125" customWidth="1"/>
+    <col min="28" max="28" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:29">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:29">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -841,7 +1388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:29">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -849,424 +1396,1085 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:29">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="H12" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
+      <c r="P11" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="32"/>
+      <c r="W11" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="X11" s="32"/>
+      <c r="AA11" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB11" s="32"/>
+    </row>
+    <row r="12" spans="1:29">
+      <c r="A12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="10" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="33"/>
+      <c r="T12" s="33"/>
+      <c r="U12" s="33"/>
+      <c r="W12" s="33"/>
+      <c r="X12" s="33"/>
+      <c r="AA12" s="33"/>
+      <c r="AB12" s="33"/>
+    </row>
+    <row r="13" spans="1:29" ht="26">
+      <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>48</v>
+      <c r="B13" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>34</v>
+      </c>
+      <c r="P13" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="S13" s="21"/>
+      <c r="T13" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="U13" s="21"/>
+      <c r="W13" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="X13" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA13" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB13" s="52" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="16" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="8" t="s">
+      <c r="B14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="P14" s="19"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="36"/>
+      <c r="U14" s="37"/>
+      <c r="X14" s="36"/>
+      <c r="AB14" s="36"/>
+    </row>
+    <row r="15" spans="1:29" ht="21">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="S15" s="39"/>
+      <c r="T15" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="U15" s="46"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y15" s="24"/>
+      <c r="Z15" s="24"/>
+      <c r="AA15" s="24"/>
+      <c r="AB15" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC15" s="24"/>
+    </row>
+    <row r="16" spans="1:29" ht="16" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="S16" s="31"/>
+      <c r="T16" s="47"/>
+      <c r="U16" s="48"/>
+      <c r="V16" s="24"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="47"/>
+      <c r="Y16" s="24"/>
+      <c r="Z16" s="24"/>
+      <c r="AA16" s="24"/>
+      <c r="AB16" s="47"/>
+      <c r="AC16" s="24"/>
+    </row>
+    <row r="17" spans="1:29">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="I17" s="8"/>
+      <c r="P17" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="U17" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="V17" s="24"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="47"/>
+      <c r="Y17" s="24"/>
+      <c r="Z17" s="24"/>
+      <c r="AA17" s="24"/>
+      <c r="AB17" s="47"/>
+      <c r="AC17" s="24"/>
+    </row>
+    <row r="18" spans="1:29">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="H18" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H18" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="H19" s="9" t="s">
+      <c r="P18" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="47"/>
+      <c r="U18" s="48"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y18" s="24"/>
+      <c r="Z18" s="24"/>
+      <c r="AA18" s="24"/>
+      <c r="AB18" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC18" s="24"/>
+    </row>
+    <row r="19" spans="1:29">
+      <c r="H19" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="P19" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="U19" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="V19" s="24"/>
+      <c r="W19" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="X19" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y19" s="24"/>
+      <c r="Z19" s="24"/>
+      <c r="AA19" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB19" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC19" s="24"/>
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H20" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="P20" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q20" s="41"/>
+      <c r="R20" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="S20" s="44"/>
+      <c r="T20" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="U20" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="V20" s="24"/>
+      <c r="W20" s="24"/>
+      <c r="X20" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y20" s="24"/>
+      <c r="Z20" s="24"/>
+      <c r="AA20" s="24"/>
+      <c r="AB20" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC20" s="24"/>
+    </row>
+    <row r="21" spans="1:29">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B21" t="s">
+        <v>125</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="P21" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q21" s="42"/>
+      <c r="R21" s="43"/>
+      <c r="S21" s="44"/>
+      <c r="T21" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="U21" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="V21" s="24"/>
+      <c r="W21" s="24"/>
+      <c r="X21" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y21" s="24"/>
+      <c r="Z21" s="24"/>
+      <c r="AA21" s="24"/>
+      <c r="AB21" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC21" s="24"/>
+    </row>
+    <row r="22" spans="1:29" ht="16" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>48</v>
+      </c>
+      <c r="P22" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q22" s="30"/>
+      <c r="R22" s="43"/>
+      <c r="S22" s="44"/>
+      <c r="T22" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="U22" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="V22" s="24"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y22" s="24"/>
+      <c r="Z22" s="24"/>
+      <c r="AA22" s="24"/>
+      <c r="AB22" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC22" s="24"/>
+    </row>
+    <row r="23" spans="1:29">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>119</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="43"/>
+      <c r="S23" s="44"/>
+      <c r="T23" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="U23" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="V23" s="24"/>
+      <c r="W23" s="24"/>
+      <c r="X23" s="51"/>
+      <c r="Y23" s="24"/>
+      <c r="Z23" s="24"/>
+      <c r="AA23" s="24"/>
+      <c r="AB23" s="47"/>
+      <c r="AC23" s="24"/>
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
       </c>
       <c r="H24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>41</v>
+      </c>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="43"/>
+      <c r="S24" s="44"/>
+      <c r="T24" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="U24" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="V24" s="24"/>
+      <c r="W24" s="24"/>
+      <c r="X24" s="47"/>
+      <c r="Y24" s="24"/>
+      <c r="Z24" s="24"/>
+      <c r="AA24" s="24"/>
+      <c r="AB24" s="47"/>
+      <c r="AC24" s="24"/>
+    </row>
+    <row r="25" spans="1:29">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="R25" s="36"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="36"/>
+      <c r="U25" s="37"/>
+      <c r="X25" s="36"/>
+      <c r="AB25" s="36"/>
+    </row>
+    <row r="26" spans="1:29">
       <c r="A26" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>38</v>
+      </c>
+      <c r="AB26" s="37"/>
+    </row>
+    <row r="27" spans="1:29">
       <c r="H27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>54</v>
+      </c>
+      <c r="P27" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q27" s="32"/>
+      <c r="T27" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="U27" s="32"/>
+      <c r="W27" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="X27" s="32"/>
+      <c r="AA27" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB27" s="32"/>
+    </row>
+    <row r="28" spans="1:29">
       <c r="A28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H28" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="P28" s="33"/>
+      <c r="Q28" s="33"/>
+      <c r="T28" s="33"/>
+      <c r="U28" s="33"/>
+      <c r="W28" s="33"/>
+      <c r="X28" s="33"/>
+      <c r="AA28" s="33"/>
+      <c r="AB28" s="33"/>
+    </row>
+    <row r="29" spans="1:29" ht="26">
       <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="H29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>42</v>
+      </c>
+      <c r="P29" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q29" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="T29" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="U29" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="W29" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="X29" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA29" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB29" s="52" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="Q30" s="36"/>
+      <c r="U30" s="36"/>
+      <c r="X30" s="36"/>
+      <c r="AB30" s="36"/>
+    </row>
+    <row r="31" spans="1:29" ht="21">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>120</v>
+      </c>
+      <c r="Q31" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="U31" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="X31" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB31" s="53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29">
       <c r="A32" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
         <v>17</v>
       </c>
-      <c r="H32" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="I32" s="6"/>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="H32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="Q32" s="36"/>
+      <c r="U32" s="36"/>
+      <c r="X32" s="36"/>
+      <c r="AB32" s="36"/>
+    </row>
+    <row r="33" spans="1:28">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B33" t="s">
         <v>18</v>
       </c>
-      <c r="H33" s="7" t="s">
+      <c r="H33" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q33" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="U33" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="X33" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB33" s="51" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:28">
       <c r="A34" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
-      </c>
-      <c r="H34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q34" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="U34" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="X34" s="51" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="H35" s="13" t="s">
+      <c r="AB34" s="51" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="35" spans="1:28">
+      <c r="H35" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q35" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="T35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U35" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="W35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="X35" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB35" s="51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28">
       <c r="A36" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H36" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="H36" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q36" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="U36" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="X36" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB36" s="51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28">
       <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>125</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q37" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="U37" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="X37" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB37" s="51" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28">
       <c r="A38" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>49</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q38" s="36"/>
+      <c r="U38" s="36"/>
+      <c r="X38" s="36"/>
+      <c r="AB38" s="36"/>
+    </row>
+    <row r="39" spans="1:28">
       <c r="A39" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
-      </c>
-      <c r="H39" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>121</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q39" s="36"/>
+      <c r="U39" s="36"/>
+      <c r="X39" s="36"/>
+      <c r="AB39" s="36"/>
+    </row>
+    <row r="40" spans="1:28">
       <c r="A40" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B40" t="s">
         <v>17</v>
       </c>
-      <c r="H40" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="H40" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q40" s="36"/>
+      <c r="U40" s="36"/>
+      <c r="X40" s="36"/>
+      <c r="AB40" s="36"/>
+    </row>
+    <row r="41" spans="1:28">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B41" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+    </row>
+    <row r="42" spans="1:28">
       <c r="A42" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>35</v>
+      </c>
+      <c r="H42" t="s">
+        <v>69</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J42" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K42" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L42" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M42" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="N42" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28">
+      <c r="H43" s="54" t="s">
+        <v>126</v>
+      </c>
+      <c r="I43" t="s">
+        <v>77</v>
+      </c>
+      <c r="J43" t="s">
+        <v>82</v>
+      </c>
+      <c r="K43" t="s">
+        <v>87</v>
+      </c>
+      <c r="L43" t="s">
+        <v>92</v>
+      </c>
+      <c r="M43" t="s">
+        <v>58</v>
+      </c>
+      <c r="N43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28">
       <c r="A44" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="H44" s="14"/>
+      <c r="I44" t="s">
+        <v>78</v>
+      </c>
+      <c r="J44" t="s">
+        <v>83</v>
+      </c>
+      <c r="K44" t="s">
+        <v>88</v>
+      </c>
+      <c r="L44" t="s">
+        <v>93</v>
+      </c>
+      <c r="M44" t="s">
+        <v>60</v>
+      </c>
+      <c r="N44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28">
       <c r="A45" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>125</v>
+      </c>
+      <c r="H45" s="14"/>
+      <c r="I45" t="s">
+        <v>79</v>
+      </c>
+      <c r="J45" t="s">
+        <v>84</v>
+      </c>
+      <c r="K45" t="s">
+        <v>89</v>
+      </c>
+      <c r="L45" t="s">
+        <v>94</v>
+      </c>
+      <c r="M45" t="s">
+        <v>62</v>
+      </c>
+      <c r="N45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28">
       <c r="A46" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>47</v>
+      </c>
+      <c r="H46" s="14"/>
+      <c r="I46" t="s">
+        <v>80</v>
+      </c>
+      <c r="J46" t="s">
+        <v>85</v>
+      </c>
+      <c r="K46" t="s">
+        <v>90</v>
+      </c>
+      <c r="L46" t="s">
+        <v>95</v>
+      </c>
+      <c r="M46" t="s">
+        <v>64</v>
+      </c>
+      <c r="N46" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28">
       <c r="A47" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>122</v>
+      </c>
+      <c r="H47" s="15"/>
+      <c r="I47" t="s">
+        <v>81</v>
+      </c>
+      <c r="J47" t="s">
+        <v>86</v>
+      </c>
+      <c r="K47" t="s">
+        <v>91</v>
+      </c>
+      <c r="L47" t="s">
+        <v>96</v>
+      </c>
+      <c r="M47" t="s">
+        <v>66</v>
+      </c>
+      <c r="N47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28">
       <c r="A48" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B48" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="H48" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="I48" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="K48" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="L48" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="M48" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="N48" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B49" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="H49" s="17"/>
+      <c r="I49" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="J49" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="K49" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="L49" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="M49" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="N49" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+        <v>35</v>
+      </c>
+      <c r="H50" s="17"/>
+      <c r="I50" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="J50" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="K50" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="L50" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="M50" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="N50" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="H51" s="17"/>
+      <c r="I51" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="K51" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="L51" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="M51" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="N51" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="H52" s="17"/>
+      <c r="I52" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="K52" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L52" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="M52" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="N52" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="A54" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B54" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
       <c r="A55" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B55" t="s">
-        <v>33</v>
-      </c>
-      <c r="I55" s="4"/>
-    </row>
-    <row r="56" spans="1:9">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
       <c r="A56" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B56" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:14">
       <c r="A57" s="1" t="s">
         <v>14</v>
       </c>
@@ -1274,46 +2482,46 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:14">
       <c r="A58" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
       <c r="A60" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:14">
       <c r="A61" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
       <c r="A62" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B62" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
       <c r="A63" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B63" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
       <c r="A64" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B64" t="s">
         <v>17</v>
@@ -1332,11 +2540,33 @@
         <v>15</v>
       </c>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="26">
+    <mergeCell ref="P11:U12"/>
+    <mergeCell ref="W11:X12"/>
+    <mergeCell ref="AA11:AB12"/>
+    <mergeCell ref="P27:Q28"/>
+    <mergeCell ref="T27:U28"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="AA27:AB28"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="R16:S19"/>
+    <mergeCell ref="R20:S24"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P22:Q24"/>
+    <mergeCell ref="H43:H47"/>
+    <mergeCell ref="H48:H52"/>
+    <mergeCell ref="P13:Q13"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A12:F12"/>
     <mergeCell ref="H12:I12"/>

</xml_diff>